<commit_message>
Whitelisted some imports in scenario_editor
</commit_message>
<xml_diff>
--- a/data/outputs/solar-scenario2-updated.xlsx
+++ b/data/outputs/solar-scenario2-updated.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,7 +475,7 @@
         <v>1990</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -498,7 +498,7 @@
         <v>1995</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
         <v>2000</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -544,7 +544,7 @@
         <v>2005</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         <v>2010</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
         <v>2020</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -613,7 +613,7 @@
         <v>2030</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
         <v>2040</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
         <v>2050</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -682,7 +682,7 @@
         <v>2060</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -705,7 +705,7 @@
         <v>2070</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -728,7 +728,7 @@
         <v>2015</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
         <v>2025</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         <v>2035</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         <v>2045</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -820,7 +820,7 @@
         <v>2055</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
         <v>1990</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -866,7 +866,7 @@
         <v>1995</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
         <v>2000</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
         <v>2005</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -935,7 +935,7 @@
         <v>2010</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -958,7 +958,7 @@
         <v>2020</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
         <v>2030</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1004,7 +1004,7 @@
         <v>2040</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>2050</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
         <v>2060</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1073,7 +1073,7 @@
         <v>2070</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1096,7 +1096,7 @@
         <v>2015</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1119,7 +1119,7 @@
         <v>2025</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1142,7 +1142,7 @@
         <v>2035</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1165,7 +1165,7 @@
         <v>2045</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1188,7 +1188,7 @@
         <v>2055</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
         <v>1990</v>
       </c>
       <c r="D34" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1234,7 +1234,7 @@
         <v>1995</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>2000</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1280,7 +1280,7 @@
         <v>2005</v>
       </c>
       <c r="D37" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
         <v>2010</v>
       </c>
       <c r="D38" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1326,7 +1326,7 @@
         <v>2020</v>
       </c>
       <c r="D39" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1349,7 +1349,7 @@
         <v>2030</v>
       </c>
       <c r="D40" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         <v>2040</v>
       </c>
       <c r="D41" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1395,7 +1395,7 @@
         <v>2050</v>
       </c>
       <c r="D42" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1418,7 +1418,7 @@
         <v>2060</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1441,7 +1441,7 @@
         <v>2070</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1464,7 +1464,7 @@
         <v>2015</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>2025</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>2035</v>
       </c>
       <c r="D47" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1533,7 +1533,7 @@
         <v>2045</v>
       </c>
       <c r="D48" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1556,7 +1556,7 @@
         <v>2055</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1579,7 +1579,7 @@
         <v>1990</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1602,7 +1602,7 @@
         <v>1995</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1625,7 +1625,7 @@
         <v>2000</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1648,7 +1648,7 @@
         <v>2005</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         <v>2010</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1694,7 +1694,7 @@
         <v>2020</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>2030</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1740,7 +1740,7 @@
         <v>2040</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1763,7 +1763,7 @@
         <v>2050</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1786,7 +1786,7 @@
         <v>2060</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1809,7 +1809,7 @@
         <v>2070</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
         <v>2015</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         <v>2025</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2000000000000012</v>
+        <v>0.1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
         <v>2035</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1901,7 +1901,7 @@
         <v>2045</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1924,7 +1924,7 @@
         <v>2055</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3028,7 +3028,7 @@
         <v>1990</v>
       </c>
       <c r="D113" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3051,7 +3051,7 @@
         <v>1995</v>
       </c>
       <c r="D114" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3074,7 +3074,7 @@
         <v>2000</v>
       </c>
       <c r="D115" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
         <v>2005</v>
       </c>
       <c r="D116" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3120,7 +3120,7 @@
         <v>2010</v>
       </c>
       <c r="D117" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3143,7 +3143,7 @@
         <v>2015</v>
       </c>
       <c r="D118" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3166,7 +3166,7 @@
         <v>2020</v>
       </c>
       <c r="D119" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3189,7 +3189,7 @@
         <v>2025</v>
       </c>
       <c r="D120" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3212,7 +3212,7 @@
         <v>2030</v>
       </c>
       <c r="D121" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3235,7 +3235,7 @@
         <v>2035</v>
       </c>
       <c r="D122" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3258,7 +3258,7 @@
         <v>2040</v>
       </c>
       <c r="D123" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3281,7 +3281,7 @@
         <v>2045</v>
       </c>
       <c r="D124" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3304,7 +3304,7 @@
         <v>2050</v>
       </c>
       <c r="D125" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3327,7 +3327,7 @@
         <v>2055</v>
       </c>
       <c r="D126" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3350,7 +3350,7 @@
         <v>2060</v>
       </c>
       <c r="D127" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         <v>2070</v>
       </c>
       <c r="D128" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3396,7 +3396,7 @@
         <v>1990</v>
       </c>
       <c r="D129" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3419,7 +3419,7 @@
         <v>1995</v>
       </c>
       <c r="D130" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
         <v>2000</v>
       </c>
       <c r="D131" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3465,7 +3465,7 @@
         <v>2005</v>
       </c>
       <c r="D132" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3488,7 +3488,7 @@
         <v>2010</v>
       </c>
       <c r="D133" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3511,7 +3511,7 @@
         <v>2015</v>
       </c>
       <c r="D134" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3534,7 +3534,7 @@
         <v>2020</v>
       </c>
       <c r="D135" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3557,7 +3557,7 @@
         <v>2025</v>
       </c>
       <c r="D136" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3580,7 +3580,7 @@
         <v>2030</v>
       </c>
       <c r="D137" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
         <v>2035</v>
       </c>
       <c r="D138" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3626,7 +3626,7 @@
         <v>2040</v>
       </c>
       <c r="D139" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3649,7 +3649,7 @@
         <v>2045</v>
       </c>
       <c r="D140" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3672,7 +3672,7 @@
         <v>2050</v>
       </c>
       <c r="D141" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3695,7 +3695,7 @@
         <v>2055</v>
       </c>
       <c r="D142" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3718,7 +3718,7 @@
         <v>2060</v>
       </c>
       <c r="D143" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3741,7 +3741,7 @@
         <v>2070</v>
       </c>
       <c r="D144" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3764,7 +3764,7 @@
         <v>1990</v>
       </c>
       <c r="D145" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
         <v>1995</v>
       </c>
       <c r="D146" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -3810,7 +3810,7 @@
         <v>2000</v>
       </c>
       <c r="D147" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -3833,7 +3833,7 @@
         <v>2005</v>
       </c>
       <c r="D148" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -3856,7 +3856,7 @@
         <v>2010</v>
       </c>
       <c r="D149" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -3879,7 +3879,7 @@
         <v>2015</v>
       </c>
       <c r="D150" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -3902,7 +3902,7 @@
         <v>2020</v>
       </c>
       <c r="D151" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -3925,7 +3925,7 @@
         <v>2025</v>
       </c>
       <c r="D152" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -3948,7 +3948,7 @@
         <v>2030</v>
       </c>
       <c r="D153" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -3971,7 +3971,7 @@
         <v>2035</v>
       </c>
       <c r="D154" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -3994,7 +3994,7 @@
         <v>2040</v>
       </c>
       <c r="D155" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4017,7 +4017,7 @@
         <v>2045</v>
       </c>
       <c r="D156" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4040,7 +4040,7 @@
         <v>2050</v>
       </c>
       <c r="D157" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4063,7 +4063,7 @@
         <v>2055</v>
       </c>
       <c r="D158" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4086,7 +4086,7 @@
         <v>2060</v>
       </c>
       <c r="D159" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4109,7 +4109,7 @@
         <v>2070</v>
       </c>
       <c r="D160" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4132,7 +4132,7 @@
         <v>1990</v>
       </c>
       <c r="D161" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4155,7 +4155,7 @@
         <v>1995</v>
       </c>
       <c r="D162" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4178,7 +4178,7 @@
         <v>2000</v>
       </c>
       <c r="D163" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4201,7 +4201,7 @@
         <v>2005</v>
       </c>
       <c r="D164" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4224,7 +4224,7 @@
         <v>2010</v>
       </c>
       <c r="D165" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
         <v>2015</v>
       </c>
       <c r="D166" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4270,7 +4270,7 @@
         <v>2020</v>
       </c>
       <c r="D167" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4293,7 +4293,7 @@
         <v>2025</v>
       </c>
       <c r="D168" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4316,7 +4316,7 @@
         <v>2030</v>
       </c>
       <c r="D169" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         <v>2035</v>
       </c>
       <c r="D170" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
         <v>2040</v>
       </c>
       <c r="D171" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4385,7 +4385,7 @@
         <v>2045</v>
       </c>
       <c r="D172" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4408,7 +4408,7 @@
         <v>2050</v>
       </c>
       <c r="D173" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4431,7 +4431,7 @@
         <v>2055</v>
       </c>
       <c r="D174" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4454,7 +4454,7 @@
         <v>2060</v>
       </c>
       <c r="D175" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4477,7 +4477,7 @@
         <v>2070</v>
       </c>
       <c r="D176" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4500,7 +4500,7 @@
         <v>1990</v>
       </c>
       <c r="D177" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4523,7 +4523,7 @@
         <v>1995</v>
       </c>
       <c r="D178" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4546,7 +4546,7 @@
         <v>2000</v>
       </c>
       <c r="D179" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4569,7 +4569,7 @@
         <v>2005</v>
       </c>
       <c r="D180" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4592,7 +4592,7 @@
         <v>2010</v>
       </c>
       <c r="D181" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4615,7 +4615,7 @@
         <v>2015</v>
       </c>
       <c r="D182" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4638,7 +4638,7 @@
         <v>2020</v>
       </c>
       <c r="D183" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4661,7 +4661,7 @@
         <v>2025</v>
       </c>
       <c r="D184" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4684,7 +4684,7 @@
         <v>2030</v>
       </c>
       <c r="D185" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4707,7 +4707,7 @@
         <v>2035</v>
       </c>
       <c r="D186" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -4730,7 +4730,7 @@
         <v>2040</v>
       </c>
       <c r="D187" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -4753,7 +4753,7 @@
         <v>2045</v>
       </c>
       <c r="D188" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -4776,7 +4776,7 @@
         <v>2050</v>
       </c>
       <c r="D189" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -4799,7 +4799,7 @@
         <v>2055</v>
       </c>
       <c r="D190" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -4822,7 +4822,7 @@
         <v>2060</v>
       </c>
       <c r="D191" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -4845,7 +4845,7 @@
         <v>2070</v>
       </c>
       <c r="D192" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -4868,7 +4868,7 @@
         <v>1990</v>
       </c>
       <c r="D193" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -4891,7 +4891,7 @@
         <v>1995</v>
       </c>
       <c r="D194" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -4914,7 +4914,7 @@
         <v>2000</v>
       </c>
       <c r="D195" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -4937,7 +4937,7 @@
         <v>2005</v>
       </c>
       <c r="D196" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -4960,7 +4960,7 @@
         <v>2010</v>
       </c>
       <c r="D197" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -4983,7 +4983,7 @@
         <v>2015</v>
       </c>
       <c r="D198" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5006,7 +5006,7 @@
         <v>2020</v>
       </c>
       <c r="D199" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5029,7 +5029,7 @@
         <v>2025</v>
       </c>
       <c r="D200" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5052,7 +5052,7 @@
         <v>2030</v>
       </c>
       <c r="D201" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5075,7 +5075,7 @@
         <v>2035</v>
       </c>
       <c r="D202" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5098,7 +5098,7 @@
         <v>2040</v>
       </c>
       <c r="D203" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5121,7 +5121,7 @@
         <v>2045</v>
       </c>
       <c r="D204" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5144,7 +5144,7 @@
         <v>2050</v>
       </c>
       <c r="D205" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5167,7 +5167,7 @@
         <v>2055</v>
       </c>
       <c r="D206" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5190,7 +5190,7 @@
         <v>2060</v>
       </c>
       <c r="D207" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5213,7 +5213,7 @@
         <v>2070</v>
       </c>
       <c r="D208" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5236,7 +5236,7 @@
         <v>1990</v>
       </c>
       <c r="D209" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5259,7 +5259,7 @@
         <v>1995</v>
       </c>
       <c r="D210" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5282,7 +5282,7 @@
         <v>2000</v>
       </c>
       <c r="D211" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5305,7 +5305,7 @@
         <v>2005</v>
       </c>
       <c r="D212" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
         <v>2010</v>
       </c>
       <c r="D213" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5351,7 +5351,7 @@
         <v>2015</v>
       </c>
       <c r="D214" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5374,7 +5374,7 @@
         <v>2020</v>
       </c>
       <c r="D215" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
         <v>2025</v>
       </c>
       <c r="D216" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5420,7 +5420,7 @@
         <v>2030</v>
       </c>
       <c r="D217" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5443,7 +5443,7 @@
         <v>2035</v>
       </c>
       <c r="D218" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5466,7 +5466,7 @@
         <v>2040</v>
       </c>
       <c r="D219" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5489,7 +5489,7 @@
         <v>2045</v>
       </c>
       <c r="D220" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5512,7 +5512,7 @@
         <v>2050</v>
       </c>
       <c r="D221" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5535,7 +5535,7 @@
         <v>2055</v>
       </c>
       <c r="D222" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5558,7 +5558,7 @@
         <v>2060</v>
       </c>
       <c r="D223" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5581,7 +5581,7 @@
         <v>2070</v>
       </c>
       <c r="D224" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5604,7 +5604,7 @@
         <v>1990</v>
       </c>
       <c r="D225" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5627,7 +5627,7 @@
         <v>1995</v>
       </c>
       <c r="D226" t="n">
-        <v>1212</v>
+        <v>22.9675</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -5650,7 +5650,7 @@
         <v>2000</v>
       </c>
       <c r="D227" t="n">
-        <v>1212</v>
+        <v>45.835</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -5673,7 +5673,7 @@
         <v>2005</v>
       </c>
       <c r="D228" t="n">
-        <v>1212</v>
+        <v>68.7025</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -5696,7 +5696,7 @@
         <v>2010</v>
       </c>
       <c r="D229" t="n">
-        <v>1212</v>
+        <v>91.56999999999999</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -5719,7 +5719,7 @@
         <v>2015</v>
       </c>
       <c r="D230" t="n">
-        <v>1212</v>
+        <v>114.4375</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -5742,7 +5742,7 @@
         <v>2020</v>
       </c>
       <c r="D231" t="n">
-        <v>1212</v>
+        <v>137.305</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -5765,7 +5765,7 @@
         <v>2025</v>
       </c>
       <c r="D232" t="n">
-        <v>1148.06</v>
+        <v>160.1725</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -5788,7 +5788,7 @@
         <v>2030</v>
       </c>
       <c r="D233" t="n">
-        <v>1084.14</v>
+        <v>183.04</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -5811,7 +5811,7 @@
         <v>2035</v>
       </c>
       <c r="D234" t="n">
-        <v>1027.02</v>
+        <v>205.9075</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -5834,7 +5834,7 @@
         <v>2040</v>
       </c>
       <c r="D235" t="n">
-        <v>969.9</v>
+        <v>228.775</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -5857,7 +5857,7 @@
         <v>2045</v>
       </c>
       <c r="D236" t="n">
-        <v>921</v>
+        <v>251.6425</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -5880,7 +5880,7 @@
         <v>2050</v>
       </c>
       <c r="D237" t="n">
-        <v>872.12</v>
+        <v>274.51</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -5903,7 +5903,7 @@
         <v>2055</v>
       </c>
       <c r="D238" t="n">
-        <v>832.2</v>
+        <v>297.3775000000001</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -5926,7 +5926,7 @@
         <v>2060</v>
       </c>
       <c r="D239" t="n">
-        <v>792.3</v>
+        <v>320.245</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -5949,7 +5949,7 @@
         <v>2070</v>
       </c>
       <c r="D240" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7651,7 +7651,7 @@
         <v>2010</v>
       </c>
       <c r="D314" t="n">
-        <v>750.84</v>
+        <v>375.42</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -7674,7 +7674,7 @@
         <v>2015</v>
       </c>
       <c r="D315" t="n">
-        <v>750.84</v>
+        <v>351.5616666666667</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -7697,7 +7697,7 @@
         <v>2020</v>
       </c>
       <c r="D316" t="n">
-        <v>750.84</v>
+        <v>327.7033333333334</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -7720,7 +7720,7 @@
         <v>2025</v>
       </c>
       <c r="D317" t="n">
-        <v>639.2</v>
+        <v>303.845</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -7743,7 +7743,7 @@
         <v>2030</v>
       </c>
       <c r="D318" t="n">
-        <v>527.5599999999999</v>
+        <v>279.9866666666667</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -7766,7 +7766,7 @@
         <v>2035</v>
       </c>
       <c r="D319" t="n">
-        <v>448.96</v>
+        <v>256.1283333333333</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -7789,7 +7789,7 @@
         <v>2040</v>
       </c>
       <c r="D320" t="n">
-        <v>370.38</v>
+        <v>232.27</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -7812,7 +7812,7 @@
         <v>2045</v>
       </c>
       <c r="D321" t="n">
-        <v>318.94</v>
+        <v>208.4116666666667</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -7835,7 +7835,7 @@
         <v>2050</v>
       </c>
       <c r="D322" t="n">
-        <v>267.5</v>
+        <v>184.5533333333333</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -7858,7 +7858,7 @@
         <v>2055</v>
       </c>
       <c r="D323" t="n">
-        <v>237.42</v>
+        <v>160.695</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -7881,7 +7881,7 @@
         <v>2060</v>
       </c>
       <c r="D324" t="n">
-        <v>207.34</v>
+        <v>136.8366666666667</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -7904,7 +7904,7 @@
         <v>2070</v>
       </c>
       <c r="D325" t="n">
-        <v>178.24</v>
+        <v>89.12</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8019,7 +8019,7 @@
         <v>2015</v>
       </c>
       <c r="D330" t="n">
-        <v>1212</v>
+        <v>606</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8042,7 +8042,7 @@
         <v>2020</v>
       </c>
       <c r="D331" t="n">
-        <v>1212</v>
+        <v>584.1799999999999</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8065,7 +8065,7 @@
         <v>2025</v>
       </c>
       <c r="D332" t="n">
-        <v>1148.06</v>
+        <v>562.36</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8088,7 +8088,7 @@
         <v>2030</v>
       </c>
       <c r="D333" t="n">
-        <v>1084.14</v>
+        <v>540.54</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8111,7 +8111,7 @@
         <v>2035</v>
       </c>
       <c r="D334" t="n">
-        <v>1027.02</v>
+        <v>518.72</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8134,7 +8134,7 @@
         <v>2040</v>
       </c>
       <c r="D335" t="n">
-        <v>969.9</v>
+        <v>496.9</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8157,7 +8157,7 @@
         <v>2045</v>
       </c>
       <c r="D336" t="n">
-        <v>921</v>
+        <v>475.08</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8180,7 +8180,7 @@
         <v>2050</v>
       </c>
       <c r="D337" t="n">
-        <v>872.12</v>
+        <v>453.26</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
         <v>2055</v>
       </c>
       <c r="D338" t="n">
-        <v>832.2</v>
+        <v>431.44</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8226,7 +8226,7 @@
         <v>2060</v>
       </c>
       <c r="D339" t="n">
-        <v>792.3</v>
+        <v>409.62</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8249,7 +8249,7 @@
         <v>2070</v>
       </c>
       <c r="D340" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8272,7 +8272,7 @@
         <v>2020</v>
       </c>
       <c r="D341" t="n">
-        <v>1212</v>
+        <v>606</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8295,7 +8295,7 @@
         <v>2025</v>
       </c>
       <c r="D342" t="n">
-        <v>1148.06</v>
+        <v>581.998</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8318,7 +8318,7 @@
         <v>2030</v>
       </c>
       <c r="D343" t="n">
-        <v>1084.14</v>
+        <v>557.996</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8341,7 +8341,7 @@
         <v>2035</v>
       </c>
       <c r="D344" t="n">
-        <v>1027.02</v>
+        <v>533.994</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8364,7 +8364,7 @@
         <v>2040</v>
       </c>
       <c r="D345" t="n">
-        <v>969.9</v>
+        <v>509.992</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8387,7 +8387,7 @@
         <v>2045</v>
       </c>
       <c r="D346" t="n">
-        <v>921</v>
+        <v>485.99</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -8410,7 +8410,7 @@
         <v>2050</v>
       </c>
       <c r="D347" t="n">
-        <v>872.12</v>
+        <v>461.988</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -8433,7 +8433,7 @@
         <v>2055</v>
       </c>
       <c r="D348" t="n">
-        <v>832.2</v>
+        <v>437.986</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -8456,7 +8456,7 @@
         <v>2060</v>
       </c>
       <c r="D349" t="n">
-        <v>792.3</v>
+        <v>413.984</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -8479,7 +8479,7 @@
         <v>2070</v>
       </c>
       <c r="D350" t="n">
-        <v>731.96</v>
+        <v>365.98</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>

</xml_diff>